<commit_message>
new update to add doctors to the patient registration
</commit_message>
<xml_diff>
--- a/files/new_product.xlsx
+++ b/files/new_product.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aquacy\Documents\last\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F5BB744-A333-42AC-BC68-BB31BC2CDCC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2C8288C-3206-4861-A817-6ABB3F47FCA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{3DE7F198-3571-4E61-9DD7-4C6B0DEFD61C}"/>
+    <workbookView minimized="1" xWindow="2340" yWindow="2955" windowWidth="10860" windowHeight="7785" xr2:uid="{3DE7F198-3571-4E61-9DD7-4C6B0DEFD61C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -443,12 +443,13 @@
   <dimension ref="A1:Y3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="28" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">

</xml_diff>